<commit_message>
Weapons confured for creatures and hit locations
</commit_message>
<xml_diff>
--- a/Hit_Location_Source.xlsx
+++ b/Hit_Location_Source.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psturge\Google Drive\RuneQuest\RQG\GM_aids\Stat_blocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psturge.WARWICK\My Drive\RuneQuest\RQG\GM_aids\Stat_blocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FBB301-96AB-4238-9068-14EC40B064D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="4"/>
+    <workbookView xWindow="7140" yWindow="4350" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Humanoid" sheetId="1" r:id="rId1"/>
@@ -17,15 +18,28 @@
     <sheet name="Dragonsnail2" sheetId="4" r:id="rId3"/>
     <sheet name="Scorpionman" sheetId="3" r:id="rId4"/>
     <sheet name="Beetle" sheetId="5" r:id="rId5"/>
+    <sheet name="Wyvern" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
-  <si>
-    <r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -35,7 +49,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -45,7 +59,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -55,7 +69,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -65,7 +79,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -75,7 +89,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -85,7 +99,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -95,7 +109,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -105,7 +119,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -115,7 +129,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -125,7 +139,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -135,7 +149,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -145,7 +159,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -155,18 +169,6 @@
     </r>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>D20</t>
-  </si>
-  <si>
-    <t>Armor</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
     <t>Shell</t>
   </si>
   <si>
@@ -185,6 +187,21 @@
     <t>15–20</t>
   </si>
   <si>
+    <t>09–12</t>
+  </si>
+  <si>
+    <t>Right Head</t>
+  </si>
+  <si>
+    <t>13-16</t>
+  </si>
+  <si>
+    <t>Left Head</t>
+  </si>
+  <si>
+    <t>17-20</t>
+  </si>
+  <si>
     <t>Right Hind Leg</t>
   </si>
   <si>
@@ -242,22 +259,10 @@
     <t>19–20</t>
   </si>
   <si>
-    <t>09–12</t>
-  </si>
-  <si>
-    <t>13-16</t>
-  </si>
-  <si>
-    <t>Right Head</t>
-  </si>
-  <si>
-    <t>Left Head</t>
-  </si>
-  <si>
-    <t>17-20</t>
-  </si>
-  <si>
-    <r>
+    <t>AP</t>
+  </si>
+  <si>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -267,7 +272,10 @@
     </r>
   </si>
   <si>
-    <r>
+    <t>Right Center Leg</t>
+  </si>
+  <si>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -277,7 +285,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -287,7 +295,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -297,7 +305,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -307,7 +315,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -317,7 +325,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -327,7 +335,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -337,7 +345,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -347,7 +355,7 @@
     </r>
   </si>
   <si>
-    <r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <rPr>
         <sz val="9"/>
         <rFont val="Cambria"/>
@@ -357,26 +365,52 @@
     </r>
   </si>
   <si>
-    <t>Right Center Leg</t>
-  </si>
-  <si>
-    <t>AP</t>
+    <t>Right Leg</t>
+  </si>
+  <si>
+    <t>02-04</t>
+  </si>
+  <si>
+    <t>Left Leg</t>
+  </si>
+  <si>
+    <t>05-07</t>
+  </si>
+  <si>
+    <t>Abdomen</t>
+  </si>
+  <si>
+    <t>08-08</t>
+  </si>
+  <si>
+    <t>09-11</t>
+  </si>
+  <si>
+    <t>Right Wing</t>
+  </si>
+  <si>
+    <t>13-14</t>
+  </si>
+  <si>
+    <t>Left Wing</t>
+  </si>
+  <si>
+    <t>15-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###0;###0"/>
     <numFmt numFmtId="165" formatCode="###00;###00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
@@ -493,64 +527,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -571,9 +603,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -611,9 +643,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -648,7 +680,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,7 +715,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,7 +888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -870,65 +902,65 @@
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="17.1" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="17.1" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="17.1" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="17.1" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6">
         <v>12</v>
@@ -936,83 +968,84 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="17.1" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="17.1" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" ht="18" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" ht="15">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -1022,11 +1055,11 @@
       <c r="C2" s="15">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -1036,11 +1069,11 @@
       <c r="C3" s="16">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
@@ -1050,17 +1083,18 @@
       <c r="C4" s="11">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1069,21 +1103,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" ht="15">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -1093,59 +1127,60 @@
       <c r="C2" s="15">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C3" s="16">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C4" s="11">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5">
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1158,23 +1193,23 @@
     <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" ht="15">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -1186,9 +1221,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B3" s="14">
         <v>2</v>
@@ -1200,12 +1235,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -1214,9 +1249,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B5" s="14">
         <v>5</v>
@@ -1228,9 +1263,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B6" s="14">
         <v>6</v>
@@ -1242,12 +1277,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -1256,12 +1291,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -1270,12 +1305,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
@@ -1284,12 +1319,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -1298,12 +1333,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -1312,12 +1347,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C12" s="5">
         <v>3</v>
@@ -1326,12 +1361,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -1342,36 +1377,37 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="17" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
@@ -1383,9 +1419,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -1397,9 +1433,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" s="18">
         <v>3</v>
@@ -1411,9 +1447,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" s="18">
         <v>4</v>
@@ -1425,12 +1461,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6" s="18">
         <v>6</v>
@@ -1439,12 +1475,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" s="18">
         <v>6</v>
@@ -1453,12 +1489,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" s="18">
         <v>6</v>
@@ -1467,12 +1503,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="18">
         <v>6</v>
@@ -1481,12 +1517,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C10" s="18">
         <v>6</v>
@@ -1497,5 +1533,145 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="0">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="0">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>